<commit_message>
updated to latest, according to telegram sent by Tech. Writer
</commit_message>
<xml_diff>
--- a/storage/app/import/cn-tool-tc.xlsx
+++ b/storage/app/import/cn-tool-tc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\MeMFIS\storage\app\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7E004F-35A0-4B16-B7AE-C267089491E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B87885-5B53-42C6-9CC5-9E5C57DD51AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4005" yWindow="2430" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT TOOL TC" sheetId="11" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="64">
   <si>
     <t>EA</t>
   </si>
@@ -206,13 +206,23 @@
   </si>
   <si>
     <t>qty</t>
+  </si>
+  <si>
+    <t>28-0-2243-MZ-A</t>
+  </si>
+  <si>
+    <t>28-0-2243-MZ-B</t>
+  </si>
+  <si>
+    <t>28-0-2243-MZ-C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="13">
+  <numFmts count="14">
+    <numFmt numFmtId="5" formatCode="&quot;Rp&quot;#,##0;\-&quot;Rp&quot;#,##0"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -343,7 +353,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -381,51 +391,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -440,7 +405,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -496,8 +461,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="5" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,41 +497,35 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="3" borderId="3" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="12" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="59">
     <cellStyle name="AeE­ [0]_INQUIRY ¿?¾÷AßAø " xfId="14" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="AeE­_INQUIRY ¿?¾÷AßAø " xfId="15" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="AÞ¸¶ [0]_INQUIRY ¿?¾÷AßAø " xfId="16" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -570,8 +533,11 @@
     <cellStyle name="C?AØ_¿?¾÷CoE² " xfId="18" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="C￥AØ_¿μ¾÷CoE² " xfId="19" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Comma 2 2" xfId="56" xr:uid="{A5CF5229-F8AF-4627-828F-CE6F89E3351B}"/>
     <cellStyle name="Comma 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Comma 3 2" xfId="57" xr:uid="{11BCAEA0-E1EA-4A33-B91D-8DE4E4CF7AB1}"/>
     <cellStyle name="Comma 4" xfId="51" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Comma 4 2" xfId="58" xr:uid="{9CAD8E03-AD80-4C2D-A290-DD474C95D78A}"/>
     <cellStyle name="Comma0" xfId="20" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Currency0" xfId="21" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Date" xfId="22" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
@@ -582,6 +548,7 @@
     <cellStyle name="Normal 11 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Normal 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Normal 2 107 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 2 107 4 2" xfId="55" xr:uid="{85B298B2-A045-4DF2-A1E1-7BFFA25431EA}"/>
     <cellStyle name="Normal 2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="Normal 2 28" xfId="2" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
     <cellStyle name="Normal 2 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
@@ -897,9 +864,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -945,19 +912,19 @@
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="20">
+      <c r="C2" s="20">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="22">
         <v>42019691</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G2" s="11" t="s">
@@ -968,16 +935,16 @@
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="20">
+        <v>1</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F3" s="11" t="s">
@@ -991,16 +958,16 @@
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="11">
-        <v>1</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="21" t="s">
+      <c r="C4" s="20">
+        <v>1</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -1014,13 +981,13 @@
       <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="11">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="22" t="s">
@@ -1037,16 +1004,16 @@
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="21" t="s">
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="11" t="s">
@@ -1060,19 +1027,19 @@
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="11">
-        <v>1</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="20">
+      <c r="C7" s="20">
+        <v>1</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="22">
         <v>42019691</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -1083,16 +1050,16 @@
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="11">
-        <v>1</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="21" t="s">
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -1106,16 +1073,16 @@
       <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="21" t="s">
+      <c r="C9" s="20">
+        <v>1</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="11" t="s">
@@ -1129,13 +1096,13 @@
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="11">
-        <v>1</v>
-      </c>
-      <c r="D10" s="11" t="s">
+      <c r="C10" s="20">
+        <v>1</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="22" t="s">
@@ -1152,16 +1119,16 @@
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="11">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="21" t="s">
+      <c r="C11" s="20">
+        <v>1</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>49</v>
       </c>
       <c r="F11" s="11" t="s">
@@ -1175,19 +1142,19 @@
       <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="11">
-        <v>1</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="20">
+      <c r="C12" s="20">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="22">
         <v>42019691</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -1198,16 +1165,16 @@
       <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="11">
-        <v>1</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="21" t="s">
+      <c r="C13" s="20">
+        <v>1</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F13" s="11" t="s">
@@ -1221,16 +1188,16 @@
       <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="11">
-        <v>1</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="21" t="s">
+      <c r="C14" s="20">
+        <v>1</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F14" s="11" t="s">
@@ -1244,13 +1211,13 @@
       <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11">
-        <v>1</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="C15" s="20">
+        <v>1</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -1267,16 +1234,16 @@
       <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="11">
-        <v>1</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="21" t="s">
+      <c r="C16" s="20">
+        <v>1</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>54</v>
       </c>
       <c r="F16" s="11" t="s">
@@ -1290,19 +1257,19 @@
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="11">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="24" t="s">
+      <c r="C17" s="20">
+        <v>1</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="13" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
@@ -1313,19 +1280,19 @@
       <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="11">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="20">
+      <c r="C18" s="20">
+        <v>1</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="22">
         <v>42019691</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G18" s="11" t="s">
@@ -1336,16 +1303,16 @@
       <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="11">
-        <v>1</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="21" t="s">
+      <c r="C19" s="20">
+        <v>1</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F19" s="11" t="s">
@@ -1359,16 +1326,16 @@
       <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="11">
-        <v>1</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="21" t="s">
+      <c r="C20" s="20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F20" s="11" t="s">
@@ -1382,13 +1349,13 @@
       <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="11">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="20">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="22" t="s">
@@ -1405,16 +1372,16 @@
       <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="11">
-        <v>1</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="21" t="s">
+      <c r="C22" s="20">
+        <v>1</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="22" t="s">
         <v>51</v>
       </c>
       <c r="F22" s="11" t="s">
@@ -1428,19 +1395,19 @@
       <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="11">
-        <v>1</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="20">
+      <c r="C23" s="20">
+        <v>1</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="22">
         <v>42019691</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G23" s="11" t="s">
@@ -1451,16 +1418,16 @@
       <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="11">
-        <v>1</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="21" t="s">
+      <c r="C24" s="20">
+        <v>1</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F24" s="11" t="s">
@@ -1474,16 +1441,16 @@
       <c r="A25" s="10">
         <v>24</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="11">
-        <v>1</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="21" t="s">
+      <c r="C25" s="20">
+        <v>1</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F25" s="11" t="s">
@@ -1497,13 +1464,13 @@
       <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="11">
-        <v>1</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="20">
+        <v>1</v>
+      </c>
+      <c r="D26" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="22" t="s">
@@ -1520,16 +1487,16 @@
       <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="11">
-        <v>1</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="23" t="s">
+      <c r="C27" s="20">
+        <v>1</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>51</v>
       </c>
       <c r="F27" s="11" t="s">
@@ -1543,19 +1510,19 @@
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C28" s="11">
-        <v>1</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="20">
+      <c r="C28" s="20">
+        <v>1</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="22">
         <v>42019691</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G28" s="11" t="s">
@@ -1566,16 +1533,16 @@
       <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="11">
-        <v>1</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="21" t="s">
+      <c r="C29" s="20">
+        <v>1</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F29" s="11" t="s">
@@ -1589,16 +1556,16 @@
       <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="11">
-        <v>1</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="21" t="s">
+      <c r="C30" s="20">
+        <v>1</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="11" t="s">
@@ -1612,13 +1579,13 @@
       <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="11">
-        <v>1</v>
-      </c>
-      <c r="D31" s="11" t="s">
+      <c r="C31" s="20">
+        <v>1</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="22" t="s">
@@ -1635,16 +1602,16 @@
       <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="11">
-        <v>1</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="21" t="s">
+      <c r="C32" s="20">
+        <v>1</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="22" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="11" t="s">
@@ -1658,19 +1625,19 @@
       <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="11">
-        <v>1</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="20">
+      <c r="C33" s="20">
+        <v>1</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="22">
         <v>42019691</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G33" s="11" t="s">
@@ -1681,16 +1648,16 @@
       <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="11">
-        <v>1</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" s="21" t="s">
+      <c r="C34" s="20">
+        <v>1</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F34" s="11" t="s">
@@ -1704,16 +1671,16 @@
       <c r="A35" s="10">
         <v>34</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="11">
-        <v>1</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" s="21" t="s">
+      <c r="C35" s="20">
+        <v>1</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F35" s="11" t="s">
@@ -1727,13 +1694,13 @@
       <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="11">
-        <v>1</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="C36" s="20">
+        <v>1</v>
+      </c>
+      <c r="D36" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E36" s="22" t="s">
@@ -1750,19 +1717,19 @@
       <c r="A37" s="10">
         <v>36</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="11">
-        <v>1</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="20">
+      <c r="C37" s="20">
+        <v>1</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="22">
         <v>42019691</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G37" s="11" t="s">
@@ -1773,16 +1740,16 @@
       <c r="A38" s="10">
         <v>37</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="11">
-        <v>1</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" s="21" t="s">
+      <c r="C38" s="20">
+        <v>1</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F38" s="11" t="s">
@@ -1796,16 +1763,16 @@
       <c r="A39" s="10">
         <v>38</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="11">
-        <v>1</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="21" t="s">
+      <c r="C39" s="20">
+        <v>1</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F39" s="11" t="s">
@@ -1819,13 +1786,13 @@
       <c r="A40" s="10">
         <v>39</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="11">
-        <v>1</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="C40" s="20">
+        <v>1</v>
+      </c>
+      <c r="D40" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="22" t="s">
@@ -1842,19 +1809,19 @@
       <c r="A41" s="10">
         <v>40</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="11">
-        <v>1</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="20">
+      <c r="C41" s="20">
+        <v>1</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="22">
         <v>42019691</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G41" s="11" t="s">
@@ -1865,16 +1832,16 @@
       <c r="A42" s="10">
         <v>41</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="11">
-        <v>1</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="21" t="s">
+      <c r="C42" s="20">
+        <v>1</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F42" s="11" t="s">
@@ -1888,16 +1855,16 @@
       <c r="A43" s="10">
         <v>42</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="11">
-        <v>1</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="21" t="s">
+      <c r="C43" s="20">
+        <v>1</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F43" s="11" t="s">
@@ -1911,13 +1878,13 @@
       <c r="A44" s="10">
         <v>43</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="11">
-        <v>1</v>
-      </c>
-      <c r="D44" s="11" t="s">
+      <c r="C44" s="20">
+        <v>1</v>
+      </c>
+      <c r="D44" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E44" s="22" t="s">
@@ -1934,19 +1901,19 @@
       <c r="A45" s="10">
         <v>44</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="11">
-        <v>1</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="20">
+      <c r="C45" s="20">
+        <v>1</v>
+      </c>
+      <c r="D45" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="22">
         <v>42019691</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G45" s="11" t="s">
@@ -1957,16 +1924,16 @@
       <c r="A46" s="10">
         <v>45</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="11">
-        <v>1</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="21" t="s">
+      <c r="C46" s="20">
+        <v>1</v>
+      </c>
+      <c r="D46" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F46" s="11" t="s">
@@ -1980,16 +1947,16 @@
       <c r="A47" s="10">
         <v>46</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="11">
-        <v>1</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="21" t="s">
+      <c r="C47" s="20">
+        <v>1</v>
+      </c>
+      <c r="D47" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F47" s="11" t="s">
@@ -2003,13 +1970,13 @@
       <c r="A48" s="10">
         <v>47</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="11">
-        <v>1</v>
-      </c>
-      <c r="D48" s="11" t="s">
+      <c r="C48" s="20">
+        <v>1</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E48" s="22" t="s">
@@ -2026,16 +1993,16 @@
       <c r="A49" s="10">
         <v>48</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="11">
-        <v>1</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="21" t="s">
+      <c r="C49" s="20">
+        <v>1</v>
+      </c>
+      <c r="D49" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="22" t="s">
         <v>52</v>
       </c>
       <c r="F49" s="11" t="s">
@@ -2049,19 +2016,19 @@
       <c r="A50" s="10">
         <v>49</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="11">
-        <v>1</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="20" t="s">
+      <c r="C50" s="20">
+        <v>1</v>
+      </c>
+      <c r="D50" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G50" s="11" t="s">
@@ -2072,19 +2039,19 @@
       <c r="A51" s="10">
         <v>50</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="11">
-        <v>1</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="20">
+      <c r="C51" s="20">
+        <v>1</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="22">
         <v>42019691</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G51" s="11" t="s">
@@ -2095,16 +2062,16 @@
       <c r="A52" s="10">
         <v>51</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C52" s="11">
-        <v>1</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="21" t="s">
+      <c r="C52" s="20">
+        <v>1</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F52" s="11" t="s">
@@ -2118,16 +2085,16 @@
       <c r="A53" s="10">
         <v>52</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="11">
-        <v>1</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="21" t="s">
+      <c r="C53" s="20">
+        <v>1</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F53" s="11" t="s">
@@ -2141,13 +2108,13 @@
       <c r="A54" s="10">
         <v>53</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C54" s="11">
-        <v>1</v>
-      </c>
-      <c r="D54" s="11" t="s">
+      <c r="C54" s="20">
+        <v>1</v>
+      </c>
+      <c r="D54" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E54" s="22" t="s">
@@ -2164,19 +2131,19 @@
       <c r="A55" s="10">
         <v>54</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="11">
-        <v>1</v>
-      </c>
-      <c r="D55" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="20" t="s">
+      <c r="C55" s="20">
+        <v>1</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="15" t="s">
+      <c r="F55" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G55" s="11" t="s">
@@ -2187,19 +2154,19 @@
       <c r="A56" s="10">
         <v>55</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="11">
-        <v>1</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="20">
+      <c r="C56" s="20">
+        <v>1</v>
+      </c>
+      <c r="D56" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="22">
         <v>42019691</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G56" s="11" t="s">
@@ -2210,16 +2177,16 @@
       <c r="A57" s="10">
         <v>56</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="11">
-        <v>1</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="21" t="s">
+      <c r="C57" s="20">
+        <v>1</v>
+      </c>
+      <c r="D57" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F57" s="11" t="s">
@@ -2233,16 +2200,16 @@
       <c r="A58" s="10">
         <v>57</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="11">
-        <v>1</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E58" s="21" t="s">
+      <c r="C58" s="20">
+        <v>1</v>
+      </c>
+      <c r="D58" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E58" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F58" s="11" t="s">
@@ -2256,13 +2223,13 @@
       <c r="A59" s="10">
         <v>58</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C59" s="11">
-        <v>1</v>
-      </c>
-      <c r="D59" s="11" t="s">
+      <c r="C59" s="20">
+        <v>1</v>
+      </c>
+      <c r="D59" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E59" s="22" t="s">
@@ -2279,19 +2246,19 @@
       <c r="A60" s="10">
         <v>59</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="11">
-        <v>1</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="20" t="s">
+      <c r="C60" s="20">
+        <v>1</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F60" s="15" t="s">
+      <c r="F60" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G60" s="11" t="s">
@@ -2302,19 +2269,19 @@
       <c r="A61" s="10">
         <v>60</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="11">
-        <v>1</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E61" s="20">
+      <c r="C61" s="20">
+        <v>1</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="22">
         <v>42019691</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="F61" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G61" s="11" t="s">
@@ -2325,16 +2292,16 @@
       <c r="A62" s="10">
         <v>61</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="11">
-        <v>1</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E62" s="21" t="s">
+      <c r="C62" s="20">
+        <v>1</v>
+      </c>
+      <c r="D62" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F62" s="11" t="s">
@@ -2348,16 +2315,16 @@
       <c r="A63" s="10">
         <v>62</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C63" s="11">
-        <v>1</v>
-      </c>
-      <c r="D63" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="21" t="s">
+      <c r="C63" s="20">
+        <v>1</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F63" s="11" t="s">
@@ -2371,13 +2338,13 @@
       <c r="A64" s="10">
         <v>63</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C64" s="11">
-        <v>1</v>
-      </c>
-      <c r="D64" s="11" t="s">
+      <c r="C64" s="20">
+        <v>1</v>
+      </c>
+      <c r="D64" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E64" s="22" t="s">
@@ -2394,19 +2361,19 @@
       <c r="A65" s="10">
         <v>64</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="11">
-        <v>1</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F65" s="19" t="s">
+      <c r="C65" s="20">
+        <v>1</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F65" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G65" s="11" t="s">
@@ -2417,19 +2384,19 @@
       <c r="A66" s="10">
         <v>65</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="11">
-        <v>1</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="20">
+      <c r="C66" s="20">
+        <v>1</v>
+      </c>
+      <c r="D66" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="22">
         <v>42019691</v>
       </c>
-      <c r="F66" s="15" t="s">
+      <c r="F66" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G66" s="11" t="s">
@@ -2440,16 +2407,16 @@
       <c r="A67" s="10">
         <v>66</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C67" s="11">
-        <v>1</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" s="21" t="s">
+      <c r="C67" s="20">
+        <v>1</v>
+      </c>
+      <c r="D67" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F67" s="11" t="s">
@@ -2463,16 +2430,16 @@
       <c r="A68" s="10">
         <v>67</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C68" s="11">
-        <v>1</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="21" t="s">
+      <c r="C68" s="20">
+        <v>1</v>
+      </c>
+      <c r="D68" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F68" s="11" t="s">
@@ -2486,13 +2453,13 @@
       <c r="A69" s="10">
         <v>68</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="11">
-        <v>1</v>
-      </c>
-      <c r="D69" s="11" t="s">
+      <c r="C69" s="20">
+        <v>1</v>
+      </c>
+      <c r="D69" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E69" s="22" t="s">
@@ -2509,19 +2476,19 @@
       <c r="A70" s="10">
         <v>69</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="11">
-        <v>1</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F70" s="19" t="s">
+      <c r="C70" s="20">
+        <v>1</v>
+      </c>
+      <c r="D70" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F70" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G70" s="11" t="s">
@@ -2532,19 +2499,19 @@
       <c r="A71" s="10">
         <v>70</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C71" s="11">
-        <v>1</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="20">
+      <c r="C71" s="20">
+        <v>1</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="22">
         <v>42019691</v>
       </c>
-      <c r="F71" s="15" t="s">
+      <c r="F71" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G71" s="11" t="s">
@@ -2555,16 +2522,16 @@
       <c r="A72" s="10">
         <v>71</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C72" s="11">
-        <v>1</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72" s="21" t="s">
+      <c r="C72" s="20">
+        <v>1</v>
+      </c>
+      <c r="D72" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F72" s="11" t="s">
@@ -2578,16 +2545,16 @@
       <c r="A73" s="10">
         <v>72</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="11">
-        <v>1</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="21" t="s">
+      <c r="C73" s="20">
+        <v>1</v>
+      </c>
+      <c r="D73" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F73" s="11" t="s">
@@ -2601,13 +2568,13 @@
       <c r="A74" s="10">
         <v>73</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C74" s="11">
-        <v>1</v>
-      </c>
-      <c r="D74" s="11" t="s">
+      <c r="C74" s="20">
+        <v>1</v>
+      </c>
+      <c r="D74" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E74" s="22" t="s">
@@ -2624,19 +2591,19 @@
       <c r="A75" s="10">
         <v>74</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="11">
-        <v>1</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F75" s="19" t="s">
+      <c r="C75" s="20">
+        <v>1</v>
+      </c>
+      <c r="D75" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F75" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G75" s="11" t="s">
@@ -2647,16 +2614,16 @@
       <c r="A76" s="10">
         <v>75</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C76" s="11">
-        <v>1</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" s="21" t="s">
+      <c r="C76" s="20">
+        <v>1</v>
+      </c>
+      <c r="D76" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F76" s="11" t="s">
@@ -2670,16 +2637,16 @@
       <c r="A77" s="10">
         <v>76</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C77" s="11">
-        <v>1</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="21" t="s">
+      <c r="C77" s="20">
+        <v>1</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F77" s="11" t="s">
@@ -2693,13 +2660,13 @@
       <c r="A78" s="10">
         <v>77</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C78" s="11">
-        <v>1</v>
-      </c>
-      <c r="D78" s="11" t="s">
+      <c r="C78" s="20">
+        <v>1</v>
+      </c>
+      <c r="D78" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E78" s="22" t="s">
@@ -2716,19 +2683,19 @@
       <c r="A79" s="10">
         <v>78</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="11">
-        <v>1</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F79" s="19" t="s">
+      <c r="C79" s="20">
+        <v>1</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F79" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G79" s="11" t="s">
@@ -2739,19 +2706,19 @@
       <c r="A80" s="10">
         <v>79</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="11">
-        <v>1</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="20">
+      <c r="C80" s="20">
+        <v>1</v>
+      </c>
+      <c r="D80" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="22">
         <v>42019691</v>
       </c>
-      <c r="F80" s="15" t="s">
+      <c r="F80" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G80" s="11" t="s">
@@ -2762,16 +2729,16 @@
       <c r="A81" s="10">
         <v>80</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C81" s="11">
-        <v>1</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="21" t="s">
+      <c r="C81" s="20">
+        <v>1</v>
+      </c>
+      <c r="D81" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F81" s="11" t="s">
@@ -2785,16 +2752,16 @@
       <c r="A82" s="10">
         <v>81</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="11">
-        <v>1</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="21" t="s">
+      <c r="C82" s="20">
+        <v>1</v>
+      </c>
+      <c r="D82" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F82" s="11" t="s">
@@ -2808,13 +2775,13 @@
       <c r="A83" s="10">
         <v>82</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C83" s="11">
-        <v>1</v>
-      </c>
-      <c r="D83" s="11" t="s">
+      <c r="C83" s="20">
+        <v>1</v>
+      </c>
+      <c r="D83" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E83" s="22" t="s">
@@ -2831,19 +2798,19 @@
       <c r="A84" s="10">
         <v>83</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C84" s="11">
-        <v>1</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F84" s="19" t="s">
+      <c r="C84" s="20">
+        <v>1</v>
+      </c>
+      <c r="D84" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F84" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G84" s="11" t="s">
@@ -2854,19 +2821,19 @@
       <c r="A85" s="10">
         <v>84</v>
       </c>
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C85" s="11">
-        <v>1</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="20">
+      <c r="C85" s="20">
+        <v>1</v>
+      </c>
+      <c r="D85" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="22">
         <v>42019691</v>
       </c>
-      <c r="F85" s="15" t="s">
+      <c r="F85" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G85" s="11" t="s">
@@ -2877,16 +2844,16 @@
       <c r="A86" s="10">
         <v>85</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C86" s="11">
-        <v>1</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E86" s="21" t="s">
+      <c r="C86" s="20">
+        <v>1</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F86" s="11" t="s">
@@ -2900,16 +2867,16 @@
       <c r="A87" s="10">
         <v>86</v>
       </c>
-      <c r="B87" s="17" t="s">
+      <c r="B87" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C87" s="11">
-        <v>1</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="21" t="s">
+      <c r="C87" s="20">
+        <v>1</v>
+      </c>
+      <c r="D87" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F87" s="11" t="s">
@@ -2923,13 +2890,13 @@
       <c r="A88" s="10">
         <v>87</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C88" s="11">
-        <v>1</v>
-      </c>
-      <c r="D88" s="11" t="s">
+      <c r="C88" s="20">
+        <v>1</v>
+      </c>
+      <c r="D88" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E88" s="22" t="s">
@@ -2946,19 +2913,19 @@
       <c r="A89" s="10">
         <v>88</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C89" s="11">
-        <v>1</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F89" s="19" t="s">
+      <c r="C89" s="20">
+        <v>1</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F89" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G89" s="11" t="s">
@@ -2969,19 +2936,19 @@
       <c r="A90" s="10">
         <v>89</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C90" s="11">
-        <v>1</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="20">
+      <c r="C90" s="20">
+        <v>1</v>
+      </c>
+      <c r="D90" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="22">
         <v>42019691</v>
       </c>
-      <c r="F90" s="15" t="s">
+      <c r="F90" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G90" s="11" t="s">
@@ -2992,16 +2959,16 @@
       <c r="A91" s="10">
         <v>90</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C91" s="11">
-        <v>1</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="21" t="s">
+      <c r="C91" s="20">
+        <v>1</v>
+      </c>
+      <c r="D91" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F91" s="11" t="s">
@@ -3015,16 +2982,16 @@
       <c r="A92" s="10">
         <v>91</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C92" s="11">
-        <v>1</v>
-      </c>
-      <c r="D92" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E92" s="21" t="s">
+      <c r="C92" s="20">
+        <v>1</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F92" s="11" t="s">
@@ -3038,13 +3005,13 @@
       <c r="A93" s="10">
         <v>92</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C93" s="11">
-        <v>1</v>
-      </c>
-      <c r="D93" s="11" t="s">
+      <c r="C93" s="20">
+        <v>1</v>
+      </c>
+      <c r="D93" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="22" t="s">
@@ -3061,19 +3028,19 @@
       <c r="A94" s="10">
         <v>93</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="B94" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C94" s="11">
-        <v>1</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F94" s="19" t="s">
+      <c r="C94" s="20">
+        <v>1</v>
+      </c>
+      <c r="D94" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F94" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G94" s="11" t="s">
@@ -3084,19 +3051,19 @@
       <c r="A95" s="10">
         <v>94</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C95" s="11">
-        <v>1</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="20">
+      <c r="C95" s="20">
+        <v>1</v>
+      </c>
+      <c r="D95" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="22">
         <v>42019691</v>
       </c>
-      <c r="F95" s="15" t="s">
+      <c r="F95" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G95" s="11" t="s">
@@ -3107,16 +3074,16 @@
       <c r="A96" s="10">
         <v>95</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C96" s="11">
-        <v>1</v>
-      </c>
-      <c r="D96" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="21" t="s">
+      <c r="C96" s="20">
+        <v>1</v>
+      </c>
+      <c r="D96" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F96" s="11" t="s">
@@ -3130,16 +3097,16 @@
       <c r="A97" s="10">
         <v>96</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C97" s="11">
-        <v>1</v>
-      </c>
-      <c r="D97" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="21" t="s">
+      <c r="C97" s="20">
+        <v>1</v>
+      </c>
+      <c r="D97" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F97" s="11" t="s">
@@ -3153,13 +3120,13 @@
       <c r="A98" s="10">
         <v>97</v>
       </c>
-      <c r="B98" s="17" t="s">
+      <c r="B98" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C98" s="11">
-        <v>1</v>
-      </c>
-      <c r="D98" s="11" t="s">
+      <c r="C98" s="20">
+        <v>1</v>
+      </c>
+      <c r="D98" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E98" s="22" t="s">
@@ -3176,19 +3143,19 @@
       <c r="A99" s="10">
         <v>98</v>
       </c>
-      <c r="B99" s="17" t="s">
+      <c r="B99" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C99" s="11">
-        <v>1</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E99" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F99" s="19" t="s">
+      <c r="C99" s="20">
+        <v>1</v>
+      </c>
+      <c r="D99" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F99" s="14" t="s">
         <v>44</v>
       </c>
       <c r="G99" s="11" t="s">
@@ -3199,19 +3166,19 @@
       <c r="A100" s="10">
         <v>99</v>
       </c>
-      <c r="B100" s="17" t="s">
+      <c r="B100" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C100" s="11">
-        <v>1</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="20">
+      <c r="C100" s="20">
+        <v>1</v>
+      </c>
+      <c r="D100" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="22">
         <v>42019691</v>
       </c>
-      <c r="F100" s="15" t="s">
+      <c r="F100" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G100" s="11" t="s">
@@ -3222,16 +3189,16 @@
       <c r="A101" s="10">
         <v>100</v>
       </c>
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C101" s="11">
-        <v>1</v>
-      </c>
-      <c r="D101" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E101" s="21" t="s">
+      <c r="C101" s="20">
+        <v>1</v>
+      </c>
+      <c r="D101" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F101" s="11" t="s">
@@ -3245,16 +3212,16 @@
       <c r="A102" s="10">
         <v>101</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C102" s="11">
-        <v>1</v>
-      </c>
-      <c r="D102" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="21" t="s">
+      <c r="C102" s="20">
+        <v>1</v>
+      </c>
+      <c r="D102" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F102" s="11" t="s">
@@ -3268,13 +3235,13 @@
       <c r="A103" s="10">
         <v>102</v>
       </c>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C103" s="11">
-        <v>1</v>
-      </c>
-      <c r="D103" s="11" t="s">
+      <c r="C103" s="20">
+        <v>1</v>
+      </c>
+      <c r="D103" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E103" s="22" t="s">
@@ -3291,19 +3258,19 @@
       <c r="A104" s="10">
         <v>103</v>
       </c>
-      <c r="B104" s="18" t="s">
+      <c r="B104" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C104" s="11">
-        <v>1</v>
-      </c>
-      <c r="D104" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E104" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F104" s="19" t="s">
+      <c r="C104" s="20">
+        <v>1</v>
+      </c>
+      <c r="D104" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F104" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G104" s="11" t="s">
@@ -3314,19 +3281,19 @@
       <c r="A105" s="10">
         <v>104</v>
       </c>
-      <c r="B105" s="18" t="s">
+      <c r="B105" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C105" s="11">
-        <v>1</v>
-      </c>
-      <c r="D105" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E105" s="20">
+      <c r="C105" s="20">
+        <v>1</v>
+      </c>
+      <c r="D105" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="22">
         <v>42019691</v>
       </c>
-      <c r="F105" s="15" t="s">
+      <c r="F105" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G105" s="11" t="s">
@@ -3337,16 +3304,16 @@
       <c r="A106" s="10">
         <v>105</v>
       </c>
-      <c r="B106" s="18" t="s">
+      <c r="B106" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C106" s="11">
-        <v>1</v>
-      </c>
-      <c r="D106" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="21" t="s">
+      <c r="C106" s="20">
+        <v>1</v>
+      </c>
+      <c r="D106" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F106" s="11" t="s">
@@ -3360,16 +3327,16 @@
       <c r="A107" s="10">
         <v>106</v>
       </c>
-      <c r="B107" s="18" t="s">
+      <c r="B107" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C107" s="11">
-        <v>1</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E107" s="21" t="s">
+      <c r="C107" s="20">
+        <v>1</v>
+      </c>
+      <c r="D107" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F107" s="11" t="s">
@@ -3383,13 +3350,13 @@
       <c r="A108" s="10">
         <v>107</v>
       </c>
-      <c r="B108" s="18" t="s">
+      <c r="B108" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C108" s="11">
-        <v>1</v>
-      </c>
-      <c r="D108" s="11" t="s">
+      <c r="C108" s="20">
+        <v>1</v>
+      </c>
+      <c r="D108" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E108" s="22" t="s">
@@ -3406,19 +3373,19 @@
       <c r="A109" s="10">
         <v>108</v>
       </c>
-      <c r="B109" s="18" t="s">
+      <c r="B109" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C109" s="11">
-        <v>1</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F109" s="19" t="s">
+      <c r="C109" s="20">
+        <v>1</v>
+      </c>
+      <c r="D109" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F109" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G109" s="11" t="s">
@@ -3429,19 +3396,19 @@
       <c r="A110" s="10">
         <v>109</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C110" s="11">
-        <v>1</v>
-      </c>
-      <c r="D110" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="20">
+      <c r="C110" s="20">
+        <v>1</v>
+      </c>
+      <c r="D110" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="22">
         <v>42019691</v>
       </c>
-      <c r="F110" s="15" t="s">
+      <c r="F110" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G110" s="11" t="s">
@@ -3452,16 +3419,16 @@
       <c r="A111" s="10">
         <v>110</v>
       </c>
-      <c r="B111" s="18" t="s">
+      <c r="B111" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C111" s="11">
-        <v>1</v>
-      </c>
-      <c r="D111" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E111" s="21" t="s">
+      <c r="C111" s="20">
+        <v>1</v>
+      </c>
+      <c r="D111" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F111" s="11" t="s">
@@ -3475,16 +3442,16 @@
       <c r="A112" s="10">
         <v>111</v>
       </c>
-      <c r="B112" s="18" t="s">
+      <c r="B112" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C112" s="11">
-        <v>1</v>
-      </c>
-      <c r="D112" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="21" t="s">
+      <c r="C112" s="20">
+        <v>1</v>
+      </c>
+      <c r="D112" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F112" s="11" t="s">
@@ -3498,13 +3465,13 @@
       <c r="A113" s="10">
         <v>112</v>
       </c>
-      <c r="B113" s="18" t="s">
+      <c r="B113" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C113" s="11">
-        <v>1</v>
-      </c>
-      <c r="D113" s="11" t="s">
+      <c r="C113" s="20">
+        <v>1</v>
+      </c>
+      <c r="D113" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E113" s="22" t="s">
@@ -3521,19 +3488,19 @@
       <c r="A114" s="10">
         <v>113</v>
       </c>
-      <c r="B114" s="13" t="s">
+      <c r="B114" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C114" s="11">
-        <v>1</v>
-      </c>
-      <c r="D114" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E114" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F114" s="19" t="s">
+      <c r="C114" s="20">
+        <v>1</v>
+      </c>
+      <c r="D114" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="F114" s="14" t="s">
         <v>45</v>
       </c>
       <c r="G114" s="11" t="s">
@@ -3544,19 +3511,19 @@
       <c r="A115" s="10">
         <v>114</v>
       </c>
-      <c r="B115" s="13" t="s">
+      <c r="B115" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C115" s="11">
-        <v>1</v>
-      </c>
-      <c r="D115" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E115" s="20">
+      <c r="C115" s="20">
+        <v>1</v>
+      </c>
+      <c r="D115" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E115" s="22">
         <v>42019691</v>
       </c>
-      <c r="F115" s="15" t="s">
+      <c r="F115" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G115" s="11" t="s">
@@ -3567,16 +3534,16 @@
       <c r="A116" s="10">
         <v>115</v>
       </c>
-      <c r="B116" s="13" t="s">
+      <c r="B116" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C116" s="11">
-        <v>1</v>
-      </c>
-      <c r="D116" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E116" s="21" t="s">
+      <c r="C116" s="20">
+        <v>1</v>
+      </c>
+      <c r="D116" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F116" s="11" t="s">
@@ -3590,16 +3557,16 @@
       <c r="A117" s="10">
         <v>116</v>
       </c>
-      <c r="B117" s="13" t="s">
+      <c r="B117" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C117" s="11">
-        <v>1</v>
-      </c>
-      <c r="D117" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E117" s="21" t="s">
+      <c r="C117" s="20">
+        <v>1</v>
+      </c>
+      <c r="D117" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F117" s="11" t="s">
@@ -3613,13 +3580,13 @@
       <c r="A118" s="10">
         <v>117</v>
       </c>
-      <c r="B118" s="13" t="s">
+      <c r="B118" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C118" s="11">
-        <v>1</v>
-      </c>
-      <c r="D118" s="11" t="s">
+      <c r="C118" s="20">
+        <v>1</v>
+      </c>
+      <c r="D118" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E118" s="22" t="s">
@@ -3636,19 +3603,19 @@
       <c r="A119" s="10">
         <v>118</v>
       </c>
-      <c r="B119" s="13" t="s">
+      <c r="B119" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C119" s="11">
-        <v>1</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E119" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F119" s="15" t="s">
+      <c r="C119" s="20">
+        <v>1</v>
+      </c>
+      <c r="D119" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E119" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F119" s="13" t="s">
         <v>46</v>
       </c>
       <c r="G119" s="11" t="s">
@@ -3659,19 +3626,19 @@
       <c r="A120" s="10">
         <v>119</v>
       </c>
-      <c r="B120" s="13" t="s">
+      <c r="B120" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C120" s="11">
-        <v>1</v>
-      </c>
-      <c r="D120" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E120" s="20">
+      <c r="C120" s="20">
+        <v>1</v>
+      </c>
+      <c r="D120" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E120" s="22">
         <v>42019691</v>
       </c>
-      <c r="F120" s="15" t="s">
+      <c r="F120" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G120" s="11" t="s">
@@ -3682,16 +3649,16 @@
       <c r="A121" s="10">
         <v>120</v>
       </c>
-      <c r="B121" s="13" t="s">
+      <c r="B121" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C121" s="11">
-        <v>1</v>
-      </c>
-      <c r="D121" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E121" s="21" t="s">
+      <c r="C121" s="20">
+        <v>1</v>
+      </c>
+      <c r="D121" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E121" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F121" s="11" t="s">
@@ -3705,16 +3672,16 @@
       <c r="A122" s="10">
         <v>121</v>
       </c>
-      <c r="B122" s="13" t="s">
+      <c r="B122" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C122" s="11">
-        <v>1</v>
-      </c>
-      <c r="D122" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E122" s="21" t="s">
+      <c r="C122" s="20">
+        <v>1</v>
+      </c>
+      <c r="D122" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F122" s="11" t="s">
@@ -3728,13 +3695,13 @@
       <c r="A123" s="10">
         <v>122</v>
       </c>
-      <c r="B123" s="13" t="s">
+      <c r="B123" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C123" s="11">
-        <v>1</v>
-      </c>
-      <c r="D123" s="11" t="s">
+      <c r="C123" s="20">
+        <v>1</v>
+      </c>
+      <c r="D123" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E123" s="22" t="s">
@@ -3751,19 +3718,19 @@
       <c r="A124" s="10">
         <v>123</v>
       </c>
-      <c r="B124" s="13" t="s">
+      <c r="B124" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C124" s="11">
-        <v>1</v>
-      </c>
-      <c r="D124" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E124" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F124" s="15" t="s">
+      <c r="C124" s="20">
+        <v>1</v>
+      </c>
+      <c r="D124" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E124" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F124" s="13" t="s">
         <v>46</v>
       </c>
       <c r="G124" s="11" t="s">
@@ -3774,19 +3741,19 @@
       <c r="A125" s="10">
         <v>124</v>
       </c>
-      <c r="B125" s="13" t="s">
+      <c r="B125" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C125" s="11">
-        <v>1</v>
-      </c>
-      <c r="D125" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E125" s="20">
+      <c r="C125" s="20">
+        <v>1</v>
+      </c>
+      <c r="D125" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E125" s="22">
         <v>42019691</v>
       </c>
-      <c r="F125" s="15" t="s">
+      <c r="F125" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G125" s="11" t="s">
@@ -3797,16 +3764,16 @@
       <c r="A126" s="10">
         <v>125</v>
       </c>
-      <c r="B126" s="13" t="s">
+      <c r="B126" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C126" s="11">
-        <v>1</v>
-      </c>
-      <c r="D126" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E126" s="21" t="s">
+      <c r="C126" s="20">
+        <v>1</v>
+      </c>
+      <c r="D126" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E126" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F126" s="11" t="s">
@@ -3820,16 +3787,16 @@
       <c r="A127" s="10">
         <v>126</v>
       </c>
-      <c r="B127" s="13" t="s">
+      <c r="B127" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C127" s="11">
-        <v>1</v>
-      </c>
-      <c r="D127" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E127" s="21" t="s">
+      <c r="C127" s="20">
+        <v>1</v>
+      </c>
+      <c r="D127" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E127" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F127" s="11" t="s">
@@ -3843,13 +3810,13 @@
       <c r="A128" s="10">
         <v>127</v>
       </c>
-      <c r="B128" s="13" t="s">
+      <c r="B128" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C128" s="11">
-        <v>1</v>
-      </c>
-      <c r="D128" s="11" t="s">
+      <c r="C128" s="20">
+        <v>1</v>
+      </c>
+      <c r="D128" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E128" s="22" t="s">
@@ -3866,19 +3833,19 @@
       <c r="A129" s="10">
         <v>128</v>
       </c>
-      <c r="B129" s="13" t="s">
+      <c r="B129" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C129" s="11">
-        <v>1</v>
-      </c>
-      <c r="D129" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E129" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F129" s="15" t="s">
+      <c r="C129" s="20">
+        <v>1</v>
+      </c>
+      <c r="D129" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E129" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F129" s="13" t="s">
         <v>46</v>
       </c>
       <c r="G129" s="11" t="s">
@@ -3889,19 +3856,19 @@
       <c r="A130" s="10">
         <v>129</v>
       </c>
-      <c r="B130" s="13" t="s">
+      <c r="B130" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C130" s="11">
-        <v>1</v>
-      </c>
-      <c r="D130" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E130" s="20">
+      <c r="C130" s="20">
+        <v>1</v>
+      </c>
+      <c r="D130" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E130" s="22">
         <v>42019691</v>
       </c>
-      <c r="F130" s="15" t="s">
+      <c r="F130" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G130" s="11" t="s">
@@ -3912,16 +3879,16 @@
       <c r="A131" s="10">
         <v>130</v>
       </c>
-      <c r="B131" s="13" t="s">
+      <c r="B131" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C131" s="11">
-        <v>1</v>
-      </c>
-      <c r="D131" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E131" s="21" t="s">
+      <c r="C131" s="20">
+        <v>1</v>
+      </c>
+      <c r="D131" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E131" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F131" s="11" t="s">
@@ -3935,16 +3902,16 @@
       <c r="A132" s="10">
         <v>131</v>
       </c>
-      <c r="B132" s="13" t="s">
+      <c r="B132" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C132" s="11">
-        <v>1</v>
-      </c>
-      <c r="D132" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E132" s="21" t="s">
+      <c r="C132" s="20">
+        <v>1</v>
+      </c>
+      <c r="D132" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E132" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F132" s="11" t="s">
@@ -3958,13 +3925,13 @@
       <c r="A133" s="10">
         <v>132</v>
       </c>
-      <c r="B133" s="13" t="s">
+      <c r="B133" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C133" s="11">
-        <v>1</v>
-      </c>
-      <c r="D133" s="11" t="s">
+      <c r="C133" s="20">
+        <v>1</v>
+      </c>
+      <c r="D133" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E133" s="22" t="s">
@@ -3981,19 +3948,19 @@
       <c r="A134" s="10">
         <v>133</v>
       </c>
-      <c r="B134" s="13" t="s">
+      <c r="B134" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C134" s="11">
-        <v>1</v>
-      </c>
-      <c r="D134" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E134" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F134" s="15" t="s">
+      <c r="C134" s="20">
+        <v>1</v>
+      </c>
+      <c r="D134" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E134" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F134" s="13" t="s">
         <v>46</v>
       </c>
       <c r="G134" s="11" t="s">
@@ -4004,19 +3971,19 @@
       <c r="A135" s="10">
         <v>134</v>
       </c>
-      <c r="B135" s="13" t="s">
+      <c r="B135" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C135" s="11">
-        <v>1</v>
-      </c>
-      <c r="D135" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E135" s="20">
+      <c r="C135" s="20">
+        <v>1</v>
+      </c>
+      <c r="D135" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E135" s="22">
         <v>42019691</v>
       </c>
-      <c r="F135" s="15" t="s">
+      <c r="F135" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G135" s="11" t="s">
@@ -4027,16 +3994,16 @@
       <c r="A136" s="10">
         <v>135</v>
       </c>
-      <c r="B136" s="13" t="s">
+      <c r="B136" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C136" s="11">
-        <v>1</v>
-      </c>
-      <c r="D136" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E136" s="21" t="s">
+      <c r="C136" s="20">
+        <v>1</v>
+      </c>
+      <c r="D136" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E136" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F136" s="11" t="s">
@@ -4050,16 +4017,16 @@
       <c r="A137" s="10">
         <v>136</v>
       </c>
-      <c r="B137" s="13" t="s">
+      <c r="B137" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C137" s="11">
-        <v>1</v>
-      </c>
-      <c r="D137" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E137" s="21" t="s">
+      <c r="C137" s="20">
+        <v>1</v>
+      </c>
+      <c r="D137" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E137" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F137" s="11" t="s">
@@ -4073,13 +4040,13 @@
       <c r="A138" s="10">
         <v>137</v>
       </c>
-      <c r="B138" s="13" t="s">
+      <c r="B138" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C138" s="11">
-        <v>1</v>
-      </c>
-      <c r="D138" s="11" t="s">
+      <c r="C138" s="20">
+        <v>1</v>
+      </c>
+      <c r="D138" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E138" s="22" t="s">
@@ -4096,19 +4063,19 @@
       <c r="A139" s="10">
         <v>138</v>
       </c>
-      <c r="B139" s="13" t="s">
+      <c r="B139" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C139" s="11">
-        <v>1</v>
-      </c>
-      <c r="D139" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E139" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F139" s="15" t="s">
+      <c r="C139" s="20">
+        <v>1</v>
+      </c>
+      <c r="D139" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E139" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F139" s="13" t="s">
         <v>46</v>
       </c>
       <c r="G139" s="11" t="s">
@@ -4119,19 +4086,19 @@
       <c r="A140" s="10">
         <v>139</v>
       </c>
-      <c r="B140" s="13" t="s">
+      <c r="B140" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C140" s="11">
-        <v>1</v>
-      </c>
-      <c r="D140" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E140" s="20">
+      <c r="C140" s="20">
+        <v>1</v>
+      </c>
+      <c r="D140" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E140" s="22">
         <v>42019691</v>
       </c>
-      <c r="F140" s="15" t="s">
+      <c r="F140" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G140" s="11" t="s">
@@ -4142,16 +4109,16 @@
       <c r="A141" s="10">
         <v>140</v>
       </c>
-      <c r="B141" s="13" t="s">
+      <c r="B141" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C141" s="11">
-        <v>1</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E141" s="21" t="s">
+      <c r="C141" s="20">
+        <v>1</v>
+      </c>
+      <c r="D141" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E141" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F141" s="11" t="s">
@@ -4165,16 +4132,16 @@
       <c r="A142" s="10">
         <v>141</v>
       </c>
-      <c r="B142" s="13" t="s">
+      <c r="B142" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C142" s="11">
-        <v>1</v>
-      </c>
-      <c r="D142" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E142" s="21" t="s">
+      <c r="C142" s="20">
+        <v>1</v>
+      </c>
+      <c r="D142" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E142" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F142" s="11" t="s">
@@ -4188,13 +4155,13 @@
       <c r="A143" s="10">
         <v>142</v>
       </c>
-      <c r="B143" s="13" t="s">
+      <c r="B143" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C143" s="11">
-        <v>1</v>
-      </c>
-      <c r="D143" s="11" t="s">
+      <c r="C143" s="20">
+        <v>1</v>
+      </c>
+      <c r="D143" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E143" s="22" t="s">
@@ -4211,19 +4178,19 @@
       <c r="A144" s="10">
         <v>143</v>
       </c>
-      <c r="B144" s="13" t="s">
+      <c r="B144" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C144" s="11">
-        <v>1</v>
-      </c>
-      <c r="D144" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E144" s="20">
+      <c r="C144" s="20">
+        <v>1</v>
+      </c>
+      <c r="D144" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E144" s="22">
         <v>42019691</v>
       </c>
-      <c r="F144" s="15" t="s">
+      <c r="F144" s="13" t="s">
         <v>34</v>
       </c>
       <c r="G144" s="11" t="s">
@@ -4234,16 +4201,16 @@
       <c r="A145" s="10">
         <v>144</v>
       </c>
-      <c r="B145" s="13" t="s">
+      <c r="B145" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C145" s="11">
-        <v>1</v>
-      </c>
-      <c r="D145" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E145" s="21" t="s">
+      <c r="C145" s="20">
+        <v>1</v>
+      </c>
+      <c r="D145" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E145" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F145" s="11" t="s">
@@ -4257,16 +4224,16 @@
       <c r="A146" s="10">
         <v>145</v>
       </c>
-      <c r="B146" s="13" t="s">
+      <c r="B146" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C146" s="11">
-        <v>1</v>
-      </c>
-      <c r="D146" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E146" s="21" t="s">
+      <c r="C146" s="20">
+        <v>1</v>
+      </c>
+      <c r="D146" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E146" s="22" t="s">
         <v>50</v>
       </c>
       <c r="F146" s="11" t="s">
@@ -4280,13 +4247,13 @@
       <c r="A147" s="10">
         <v>146</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C147" s="11">
-        <v>1</v>
-      </c>
-      <c r="D147" s="11" t="s">
+      <c r="C147" s="20">
+        <v>1</v>
+      </c>
+      <c r="D147" s="21" t="s">
         <v>0</v>
       </c>
       <c r="E147" s="22" t="s">

</xml_diff>